<commit_message>
make item stick to bottom
</commit_message>
<xml_diff>
--- a/back-end/utils/tutors.xlsx
+++ b/back-end/utils/tutors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\plattsburgh\coding_hub\tutoring-hub\back-end\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E5B0CB-2876-4699-A91F-5E978CF83014}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234C8F00-1042-4AEE-B599-CFBA0EBCBE9F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6A34A8B6-7C87-4F83-9E55-70AE69275A3E}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>MAT224</t>
   </si>
   <si>
-    <t>MAT225DNP</t>
-  </si>
-  <si>
     <t>MAT326</t>
   </si>
   <si>
@@ -96,12 +93,6 @@
     <t>CHE111</t>
   </si>
   <si>
-    <t>MAT102DNP</t>
-  </si>
-  <si>
-    <t>MAT221DNP</t>
-  </si>
-  <si>
     <t>PSY101</t>
   </si>
   <si>
@@ -144,9 +135,6 @@
     <t>BIO102</t>
   </si>
   <si>
-    <t>MAT161DNP</t>
-  </si>
-  <si>
     <t>Amendolia</t>
   </si>
   <si>
@@ -219,9 +207,6 @@
     <t>MAT161</t>
   </si>
   <si>
-    <t>MAT101DNP</t>
-  </si>
-  <si>
     <t>MAT108</t>
   </si>
   <si>
@@ -267,9 +252,6 @@
     <t>Franquiz</t>
   </si>
   <si>
-    <t>CSC221 DNP</t>
-  </si>
-  <si>
     <t>Carvalho</t>
   </si>
   <si>
@@ -291,9 +273,6 @@
     <t>Jennifer</t>
   </si>
   <si>
-    <t>APT101DNP</t>
-  </si>
-  <si>
     <t>PHY111</t>
   </si>
   <si>
@@ -324,9 +303,6 @@
     <t>Lam Hoang</t>
   </si>
   <si>
-    <t>ECO110DNP</t>
-  </si>
-  <si>
     <t>MGM350</t>
   </si>
   <si>
@@ -480,9 +456,6 @@
     <t>Asiya</t>
   </si>
   <si>
-    <t>ECO260 DNP</t>
-  </si>
-  <si>
     <t>Keating</t>
   </si>
   <si>
@@ -522,9 +495,6 @@
     <t>Khac Huy Ho</t>
   </si>
   <si>
-    <t>ECO260DNP</t>
-  </si>
-  <si>
     <t>Khanh Linh T. (Linh)</t>
   </si>
   <si>
@@ -651,12 +621,6 @@
     <t>Tung Hai Ngan (Daniel)</t>
   </si>
   <si>
-    <t>MAT104DNP</t>
-  </si>
-  <si>
-    <t>MAT224DNP</t>
-  </si>
-  <si>
     <t>CHE421</t>
   </si>
   <si>
@@ -753,12 +717,6 @@
     <t>Lucy</t>
   </si>
   <si>
-    <t>BIO100DNP</t>
-  </si>
-  <si>
-    <t>BIO103DNP</t>
-  </si>
-  <si>
     <t>Yeaple</t>
   </si>
   <si>
@@ -775,6 +733,48 @@
   </si>
   <si>
     <t>Cheryth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT102 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT225 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT221 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT161 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT101 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSC221  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">APT101 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECO110 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECO260  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECO260 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT104 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAT224 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIO100 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIO103 </t>
   </si>
 </sst>
 </file>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE74FF8-B07E-4E81-9C30-02ECB08CD19A}">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C79"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,48 +1294,48 @@
         <v>14</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C3" s="5">
         <v>43355</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="5">
         <v>43160</v>
@@ -1347,37 +1347,37 @@
         <v>13</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5">
         <v>43538</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>12</v>
@@ -1392,19 +1392,19 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5">
         <v>43133</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>37</v>
+        <v>237</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1414,22 +1414,22 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C7" s="5">
         <v>43349</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -1438,19 +1438,19 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C8" s="5">
         <v>43350</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1460,25 +1460,25 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5">
         <v>43508</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>12</v>
@@ -1490,98 +1490,98 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5">
         <v>42976</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C11" s="5">
         <v>43160</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>62</v>
+        <v>238</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>22</v>
+        <v>236</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C12" s="5">
         <v>43538</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C13" s="5">
         <v>43350</v>
@@ -1590,39 +1590,39 @@
         <v>12</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C14" s="5">
         <v>42997</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1632,10 +1632,10 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C15" s="5">
         <v>42437</v>
@@ -1647,27 +1647,27 @@
         <v>13</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>78</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C16" s="5">
         <v>43502</v>
@@ -1682,22 +1682,22 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C17" s="5">
         <v>42776</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>21</v>
+        <v>234</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1706,54 +1706,54 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C18" s="5">
         <v>42467</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>86</v>
+        <v>240</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C19" s="5">
         <v>43347</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1762,10 +1762,10 @@
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C20" s="5">
         <v>42975</v>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C21" s="5">
         <v>42768</v>
@@ -1795,57 +1795,57 @@
         <v>13</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>97</v>
+        <v>241</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C22" s="5">
         <v>42991</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C23" s="5">
         <v>43502</v>
@@ -1860,74 +1860,74 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C24" s="5">
         <v>43341</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C25" s="5">
         <v>43355</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C26" s="5">
         <v>42984</v>
@@ -1942,19 +1942,19 @@
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C27" s="5">
         <v>43403</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -1964,10 +1964,10 @@
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C28" s="5">
         <v>43502</v>
@@ -1982,16 +1982,16 @@
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C29" s="5">
         <v>43385</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>12</v>
@@ -2000,33 +2000,33 @@
         <v>13</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C30" s="5">
         <v>43355</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
@@ -2036,22 +2036,22 @@
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C31" s="5">
         <v>43357</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -2060,22 +2060,22 @@
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C32" s="5">
         <v>43361</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -2084,25 +2084,25 @@
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C33" s="5">
         <v>43147</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>97</v>
+        <v>241</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2110,22 +2110,22 @@
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C34" s="5">
         <v>42768</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -2134,10 +2134,10 @@
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C35" s="5">
         <v>43343</v>
@@ -2152,19 +2152,19 @@
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C36" s="5">
         <v>43353</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
@@ -2174,58 +2174,58 @@
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C37" s="5">
         <v>42783</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>149</v>
+        <v>242</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>21</v>
+        <v>234</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>22</v>
+        <v>236</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C38" s="5">
         <v>43354</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>14</v>
@@ -2234,25 +2234,25 @@
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C39" s="5">
         <v>43341</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2260,22 +2260,22 @@
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C40" s="5">
         <v>42995</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
@@ -2284,19 +2284,19 @@
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C41" s="5">
         <v>42410</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>12</v>
@@ -2305,87 +2305,87 @@
         <v>13</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>163</v>
+        <v>243</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C42" s="5">
         <v>43160</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>62</v>
+        <v>238</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>21</v>
+        <v>234</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C43" s="5">
         <v>42981</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C44" s="5">
         <v>43538</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>12</v>
@@ -2397,28 +2397,28 @@
         <v>14</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="J44" s="6"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C45" s="5">
         <v>43511</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
@@ -2428,22 +2428,22 @@
     </row>
     <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C46" s="5">
         <v>43350</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
@@ -2452,19 +2452,19 @@
     </row>
     <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C47" s="5">
         <v>42852</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
@@ -2474,19 +2474,19 @@
     </row>
     <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C48" s="5">
         <v>43403</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -2496,50 +2496,50 @@
     </row>
     <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C49" s="5">
         <v>43343</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C50" s="5">
         <v>42975</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -2548,19 +2548,19 @@
     </row>
     <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C51" s="5">
         <v>43389</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
@@ -2570,48 +2570,48 @@
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C52" s="5">
         <v>43207</v>
       </c>
       <c r="D52" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H52" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="I52" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C53" s="5">
         <v>42767</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>12</v>
@@ -2623,37 +2623,37 @@
         <v>14</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="J53" s="6"/>
     </row>
     <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C54" s="5">
         <v>42986</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>12</v>
@@ -2664,22 +2664,22 @@
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C55" s="5">
         <v>42975</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
@@ -2688,10 +2688,10 @@
     </row>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C56" s="5">
         <v>43350</v>
@@ -2706,22 +2706,22 @@
     </row>
     <row r="57" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C57" s="5">
         <v>42769</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>12</v>
@@ -2730,7 +2730,7 @@
         <v>13</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>14</v>
@@ -2738,55 +2738,55 @@
     </row>
     <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C58" s="5">
         <v>43161</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>12</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="J58" s="6"/>
     </row>
     <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C59" s="5">
         <v>43342</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -2794,52 +2794,52 @@
     </row>
     <row r="60" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C60" s="5">
         <v>42767</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>62</v>
+        <v>238</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>21</v>
+        <v>234</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>206</v>
+        <v>244</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>207</v>
+        <v>245</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="J60" s="6"/>
     </row>
     <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C61" s="5">
         <v>42626</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
@@ -2848,22 +2848,22 @@
     </row>
     <row r="62" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C62" s="5">
         <v>43342</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
@@ -2872,25 +2872,25 @@
     </row>
     <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C63" s="5">
         <v>42986</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
@@ -2898,25 +2898,25 @@
     </row>
     <row r="64" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C64" s="5">
         <v>43339</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
@@ -2924,19 +2924,19 @@
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C65" s="5">
         <v>43515</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
@@ -2946,50 +2946,50 @@
     </row>
     <row r="66" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C66" s="5">
         <v>42999</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
     </row>
     <row r="67" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C67" s="5">
         <v>43357</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
@@ -2998,16 +2998,16 @@
     </row>
     <row r="68" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C68" s="5">
         <v>43440</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
@@ -3018,22 +3018,22 @@
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C69" s="5">
         <v>42975</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
@@ -3042,68 +3042,68 @@
     </row>
     <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C70" s="5">
         <v>42419</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="J70" s="6"/>
     </row>
     <row r="71" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C71" s="5">
         <v>43340</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
     </row>
     <row r="72" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="C72" s="5">
         <v>43502</v>
@@ -3118,22 +3118,22 @@
     </row>
     <row r="73" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="C73" s="5">
         <v>43347</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G73" s="6"/>
       <c r="H73" s="6"/>
@@ -3142,16 +3142,16 @@
     </row>
     <row r="74" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="C74" s="5">
         <v>43508</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
@@ -3162,10 +3162,10 @@
     </row>
     <row r="75" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="C75" s="5">
         <v>43238</v>
@@ -3180,40 +3180,40 @@
     </row>
     <row r="76" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="C76" s="5">
         <v>43341</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="J76" s="6"/>
     </row>
     <row r="77" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="C77" s="5">
         <v>43350</v>
@@ -3225,70 +3225,70 @@
         <v>13</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J77" s="6"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="C78" s="5">
         <v>43532</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J78" s="6"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="C79" s="5">
         <v>43339</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>

</xml_diff>